<commit_message>
Trying to resolve land size class discrepancies
</commit_message>
<xml_diff>
--- a/List_Level_Codes.xlsx
+++ b/List_Level_Codes.xlsx
@@ -5,29 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Play\Statistics\SAS\2023\WorkFiles2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Play\Statistics\RStudio\NSSO-77-SAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41BDCB4-5172-4246-9BED-83D2AE63CA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6886AA0-231C-4736-88CE-501E8AB6C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61BA5D88-4AFC-4071-8CB8-965954EAF73C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Level16" sheetId="15" r:id="rId1"/>
-    <sheet name="Level15" sheetId="14" r:id="rId2"/>
-    <sheet name="Level14" sheetId="13" r:id="rId3"/>
-    <sheet name="Level13" sheetId="12" r:id="rId4"/>
-    <sheet name="Level12" sheetId="11" r:id="rId5"/>
-    <sheet name="Level11" sheetId="10" r:id="rId6"/>
-    <sheet name="Level9" sheetId="9" r:id="rId7"/>
-    <sheet name="Level8" sheetId="8" r:id="rId8"/>
-    <sheet name="Level7" sheetId="7" r:id="rId9"/>
-    <sheet name="Level6" sheetId="6" r:id="rId10"/>
-    <sheet name="Level5" sheetId="5" r:id="rId11"/>
-    <sheet name="Level4" sheetId="4" r:id="rId12"/>
-    <sheet name="Level3" sheetId="3" r:id="rId13"/>
-    <sheet name="Level2" sheetId="2" r:id="rId14"/>
-    <sheet name="Level1" sheetId="1" r:id="rId15"/>
+    <sheet name="Level19" sheetId="16" r:id="rId1"/>
+    <sheet name="Level16" sheetId="15" r:id="rId2"/>
+    <sheet name="Level15" sheetId="14" r:id="rId3"/>
+    <sheet name="Level14" sheetId="13" r:id="rId4"/>
+    <sheet name="Level13" sheetId="12" r:id="rId5"/>
+    <sheet name="Level12" sheetId="11" r:id="rId6"/>
+    <sheet name="Level11" sheetId="10" r:id="rId7"/>
+    <sheet name="Level9" sheetId="9" r:id="rId8"/>
+    <sheet name="Level8" sheetId="8" r:id="rId9"/>
+    <sheet name="Level7" sheetId="7" r:id="rId10"/>
+    <sheet name="Level6" sheetId="6" r:id="rId11"/>
+    <sheet name="Level5" sheetId="5" r:id="rId12"/>
+    <sheet name="Level4" sheetId="4" r:id="rId13"/>
+    <sheet name="Level3" sheetId="3" r:id="rId14"/>
+    <sheet name="Level2" sheetId="2" r:id="rId15"/>
+    <sheet name="Level1" sheetId="1" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="161">
   <si>
     <t>Centre code,Round,</t>
   </si>
@@ -529,6 +530,9 @@
   </si>
   <si>
     <t>Reason code</t>
+  </si>
+  <si>
+    <t>whether used for any agricultural production during July 2018- June 2019</t>
   </si>
 </sst>
 </file>
@@ -983,17 +987,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC0825-7DF9-4151-8752-71BE2A490931}">
-  <dimension ref="A1:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E964FB05-97E7-405A-9B12-C4E308C27034}">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
@@ -1124,7 +1125,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B17">
@@ -1136,28 +1137,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1165,73 +1166,121 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>76</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>77</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>78</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B28">
-        <v>57</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
-      <c r="B30">
+      <c r="B36">
         <v>10</v>
       </c>
     </row>
@@ -1241,6 +1290,269 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB3C1EA-637A-4A2D-BB39-A9D15AFF0DA9}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A1:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565D70FB-2C07-4CDA-AC65-2C319692E242}">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -1528,7 +1840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BA5CC7-6E44-48D2-9E53-731E6974AFBC}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -1751,7 +2063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67502F57-365D-4FC1-8047-76179A8807ED}">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -2089,7 +2401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286E773A-2C75-4D47-9AA7-557350CDA95C}">
   <dimension ref="A1:B42"/>
   <sheetViews>
@@ -2443,7 +2755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E6FAF2-6D9E-4C85-A7C3-F446048FCE62}">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -2741,7 +3053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4365DC-7EA8-4EC8-B888-C1C73A0A2B88}">
   <dimension ref="A1:B36"/>
   <sheetViews>
@@ -3045,6 +3357,264 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC0825-7DF9-4151-8752-71BE2A490931}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EC2BC4-7437-4A6C-A4ED-DBB9A105D606}">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -3283,7 +3853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BBA600-7A85-462F-AF8E-5BA6F59E580B}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -3506,7 +4076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD62D5B0-948C-4715-AA11-66D230261510}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -3729,7 +4299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F8E718-09D5-4149-A301-700CDEEF924C}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -3952,7 +4522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65BB175-EA1D-40FC-82B6-45C48B6DF4C6}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -4175,7 +4745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6890E785-B070-480F-89ED-228A426E9EA7}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -4390,7 +4960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2B0F6B-7A48-4D4E-8A6C-A88761909C60}">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -4627,267 +5197,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB3C1EA-637A-4A2D-BB39-A9D15AFF0DA9}">
-  <dimension ref="A1:B31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Land Size Class issue
Currently everything matches with the report
</commit_message>
<xml_diff>
--- a/List_Level_Codes.xlsx
+++ b/List_Level_Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Play\Statistics\RStudio\NSSO-77-SAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6886AA0-231C-4736-88CE-501E8AB6C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3039017-A395-4118-9915-92C2ACCE3049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61BA5D88-4AFC-4071-8CB8-965954EAF73C}"/>
   </bookViews>
@@ -618,7 +618,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -671,6 +671,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -991,7 +994,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1131,7 @@
       <c r="A17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1136,7 +1139,7 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="15">
         <v>3</v>
       </c>
     </row>
@@ -1144,7 +1147,7 @@
       <c r="A19" t="s">
         <v>70</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1152,7 +1155,7 @@
       <c r="A20" t="s">
         <v>71</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="23">
         <v>6</v>
       </c>
     </row>
@@ -1160,7 +1163,7 @@
       <c r="A21" t="s">
         <v>160</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1168,7 +1171,7 @@
       <c r="A22" t="s">
         <v>73</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1176,7 +1179,7 @@
       <c r="A23" t="s">
         <v>74</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1184,7 +1187,7 @@
       <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1192,7 +1195,7 @@
       <c r="A25" t="s">
         <v>76</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1200,7 +1203,7 @@
       <c r="A26" t="s">
         <v>77</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1208,7 +1211,7 @@
       <c r="A27" t="s">
         <v>78</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1216,7 +1219,7 @@
       <c r="A28" t="s">
         <v>79</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1224,7 +1227,7 @@
       <c r="A29" t="s">
         <v>80</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1232,7 +1235,7 @@
       <c r="A30" t="s">
         <v>81</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1240,7 +1243,7 @@
       <c r="A31" t="s">
         <v>82</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1248,7 +1251,7 @@
       <c r="A32" t="s">
         <v>83</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1256,7 +1259,7 @@
       <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1264,7 +1267,7 @@
       <c r="A34" t="s">
         <v>95</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="19">
         <v>30</v>
       </c>
     </row>
@@ -1272,7 +1275,7 @@
       <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="19">
         <v>3</v>
       </c>
     </row>
@@ -1280,7 +1283,7 @@
       <c r="A36" t="s">
         <v>31</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="20">
         <v>10</v>
       </c>
     </row>

</xml_diff>